<commit_message>
TC007 várható eredményének javítása.
</commit_message>
<xml_diff>
--- a/test/conduit_manual_test_report v100.xlsx
+++ b/test/conduit_manual_test_report v100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huske\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB396AD2-C773-4A2F-8C21-9DEF8963C6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A40E0F-5333-4994-9444-B01698CB6B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D068565-F52A-4DDA-BFFB-3E4B9E7F7DCB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{9D068565-F52A-4DDA-BFFB-3E4B9E7F7DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="117">
   <si>
     <t>Project name</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Sikeres a kijelentkezés.</t>
+  </si>
+  <si>
+    <t>Sikertelen a bejelentkezés. Megjenik az alábbi hibaüzenet: "Login failed! Password field required.".</t>
   </si>
 </sst>
 </file>
@@ -654,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -726,18 +729,79 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -758,138 +822,74 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2061,9 +2061,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A07D48F-9BA6-4879-A709-99F76122E30D}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2481,7 +2481,7 @@
       <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -2499,13 +2499,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -2520,11 +2520,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -2553,13 +2553,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
@@ -2587,11 +2587,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>81</v>
@@ -2603,11 +2603,11 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -2616,11 +2616,11 @@
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -2634,11 +2634,11 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="19"/>
       <c r="F11" s="15" t="s">
         <v>36</v>
@@ -2647,10 +2647,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -2661,93 +2661,104 @@
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="46"/>
       <c r="I14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="49"/>
+      <c r="G15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -2761,18 +2772,7 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="44" priority="1" operator="containsText" text="Medium">
@@ -2857,7 +2857,7 @@
       <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -2875,13 +2875,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -2896,11 +2896,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -2929,13 +2929,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
@@ -2963,11 +2963,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>80</v>
@@ -2979,11 +2979,11 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -2992,11 +2992,11 @@
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -3010,11 +3010,11 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="19"/>
       <c r="F11" s="15" t="s">
         <v>62</v>
@@ -3023,10 +3023,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -3037,93 +3037,104 @@
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="46"/>
       <c r="I14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="49"/>
+      <c r="G15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -3137,18 +3148,7 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Medium">
@@ -3233,7 +3233,7 @@
       <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -3251,13 +3251,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -3272,11 +3272,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -3305,13 +3305,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
@@ -3339,11 +3339,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>60</v>
@@ -3355,11 +3355,11 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -3368,11 +3368,11 @@
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -3386,11 +3386,11 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="19"/>
       <c r="F11" s="15" t="s">
         <v>36</v>
@@ -3399,10 +3399,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -3413,93 +3413,104 @@
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="46"/>
       <c r="I14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="49"/>
+      <c r="G15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -3513,18 +3524,7 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Medium">
@@ -3609,7 +3609,7 @@
       <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -3627,13 +3627,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -3648,11 +3648,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -3681,13 +3681,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
@@ -3715,11 +3715,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>54</v>
@@ -3731,11 +3731,11 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -3744,11 +3744,11 @@
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -3762,11 +3762,11 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="19"/>
       <c r="F11" s="15" t="s">
         <v>36</v>
@@ -3775,10 +3775,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -3789,93 +3789,104 @@
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="46"/>
       <c r="I14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="49"/>
+      <c r="G15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -3889,18 +3900,7 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Medium">
@@ -3985,7 +3985,7 @@
       <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -4003,13 +4003,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -4024,11 +4024,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -4057,13 +4057,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
@@ -4091,11 +4091,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>39</v>
@@ -4107,11 +4107,11 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -4120,11 +4120,11 @@
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -4138,11 +4138,11 @@
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="19"/>
       <c r="F11" s="15" t="s">
         <v>36</v>
@@ -4151,10 +4151,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -4165,99 +4165,97 @@
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="46"/>
       <c r="I14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="49"/>
+      <c r="G15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:K17"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
@@ -4273,10 +4271,12 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Medium">
@@ -4379,11 +4379,11 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -4398,11 +4398,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -4429,11 +4429,11 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -4459,11 +4459,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>35</v>
@@ -4475,24 +4475,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -4503,32 +4503,32 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="73"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -4539,110 +4539,108 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="30"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>4</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="53"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
     </row>
     <row r="20" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>5</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="30"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
@@ -4659,15 +4657,17 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="116" priority="1" operator="containsText" text="Medium">
@@ -4770,13 +4770,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -4791,11 +4791,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -4824,13 +4824,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="61">
         <v>45011</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -4858,11 +4858,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>112</v>
@@ -4874,24 +4874,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -4902,36 +4902,36 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="73"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -4942,116 +4942,136 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>4</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="80" t="s">
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="81"/>
-      <c r="G19" s="80" t="s">
+      <c r="F19" s="59"/>
+      <c r="G19" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="H19" s="81"/>
+      <c r="H19" s="59"/>
       <c r="I19" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
@@ -5064,26 +5084,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Medium">
@@ -5188,13 +5188,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -5209,11 +5209,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -5242,13 +5242,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -5276,11 +5276,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>86</v>
@@ -5292,24 +5292,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -5320,36 +5320,36 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -5360,93 +5360,113 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -5455,26 +5475,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="98" priority="1" operator="containsText" text="Medium">
@@ -5577,13 +5577,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -5598,11 +5598,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -5631,13 +5631,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -5665,11 +5665,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>99</v>
@@ -5681,24 +5681,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -5709,36 +5709,36 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -5749,93 +5749,113 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -5844,26 +5864,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Medium">
@@ -5966,13 +5966,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -5987,11 +5987,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -6020,13 +6020,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -6054,11 +6054,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>100</v>
@@ -6070,24 +6070,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -6098,36 +6098,36 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -6138,93 +6138,113 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -6233,26 +6253,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="80" priority="1" operator="containsText" text="Medium">
@@ -6355,13 +6355,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -6376,11 +6376,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -6409,13 +6409,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -6443,11 +6443,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>106</v>
@@ -6459,24 +6459,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -6487,36 +6487,36 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>71</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -6527,93 +6527,113 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -6622,26 +6642,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Medium">
@@ -6696,7 +6696,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D891D584-8F42-4990-903D-1DD4EEE39202}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6744,13 +6746,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -6765,11 +6767,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -6798,13 +6800,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>77</v>
       </c>
@@ -6832,11 +6834,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>84</v>
@@ -6848,24 +6850,24 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -6876,36 +6878,36 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>71</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -6916,93 +6918,113 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="30"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29" t="s">
+      <c r="F17" s="49"/>
+      <c r="G17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="30"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="51"/>
       <c r="I18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -7011,26 +7033,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Medium">
@@ -7133,13 +7135,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -7154,11 +7156,11 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
@@ -7187,13 +7189,13 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="70">
         <v>45011</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
@@ -7221,11 +7223,11 @@
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>82</v>
@@ -7237,20 +7239,20 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23" t="s">
         <v>34</v>
@@ -7261,34 +7263,34 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="25" t="s">
         <v>71</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="52"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="52"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -7299,66 +7301,78 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="28"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="28"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:11" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -7371,18 +7385,6 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Medium">

</xml_diff>

<commit_message>
TC_034 - Korábban létrehozott cikk sikeres törlése javítás
</commit_message>
<xml_diff>
--- a/test/conduit_manual_test_report v100.xlsx
+++ b/test/conduit_manual_test_report v100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huske\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB4B064-CE9C-4BAA-97FC-7C1F9FEA173D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA3E1E2-90C7-49A5-AEC6-71759832A276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{9D068565-F52A-4DDA-BFFB-3E4B9E7F7DCB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D068565-F52A-4DDA-BFFB-3E4B9E7F7DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2480" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="309">
   <si>
     <t>Project name</t>
   </si>
@@ -1078,6 +1078,18 @@
   </si>
   <si>
     <t>Az adatbázisban létezik az alábbi felhasználói fiók: email: piros_cica23@gmail.com password: Piroska23 továbbá létezik egy olyan felhasználó, akinek neve: FoltosCica23</t>
+  </si>
+  <si>
+    <t>A tesztelő az alábbi hivatkozásra navigál: http://localhost:1667/#/@PirosCica23/</t>
+  </si>
+  <si>
+    <t>Megjelenik a másik felhasználó profil oldala. Látható a követést szolgáló gomb</t>
+  </si>
+  <si>
+    <t>A tesztelő a "Follow PirosCica23" gombra kattint.</t>
+  </si>
+  <si>
+    <t>Megtörténik a követés, adatbázisban is nyomonkövethető. A gomb megávltozik és már a kikövetés az elérhető.</t>
   </si>
 </sst>
 </file>
@@ -5476,7 +5488,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -6122,7 +6134,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -6432,7 +6444,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
@@ -8608,9 +8620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A07D48F-9BA6-4879-A709-99F76122E30D}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9533,11 +9545,28 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="10"/>
+      <c r="A39" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B39" s="67" t="s">
+        <v>302</v>
+      </c>
+      <c r="C39" s="10" t="str" cm="1">
+        <f t="array" aca="1" ref="C39" ca="1">INDIRECT(B39&amp;"!"&amp;"D2")</f>
+        <v>Regisztrált felhasználói fiókkal egy másik létező felhasználó fiók sikeres követése.</v>
+      </c>
+      <c r="D39" s="24" t="str" cm="1">
+        <f t="array" aca="1" ref="D39" ca="1">IF(ISBLANK(INDIRECT(B39&amp;"!"&amp;"F11")),"",INDIRECT(B39&amp;"!"&amp;"F11"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="E39" s="9" t="str" cm="1">
+        <f t="array" aca="1" ref="E39" ca="1">IF(ISBLANK(INDIRECT(B39&amp;"!"&amp;"J5")),"",INDIRECT(B39&amp;"!"&amp;"J5"))</f>
+        <v>Pass</v>
+      </c>
+      <c r="F39" s="10" t="str" cm="1">
+        <f t="array" aca="1" ref="F39" ca="1">IF(ISBLANK(INDIRECT(B39&amp;"!"&amp;"H11")),"",INDIRECT(B39&amp;"!"&amp;"H11"))</f>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="9"/>
@@ -9555,7 +9584,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="containsText" dxfId="437" priority="1" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",D2)))</formula>
     </cfRule>
@@ -9620,6 +9649,7 @@
     <hyperlink ref="B36" location="TC_035!A1" display="TC_035" xr:uid="{9582A86B-32BB-4A18-9330-4B92F71F8757}"/>
     <hyperlink ref="B37" location="TC_036!A1" display="TC_036" xr:uid="{958BD88D-D688-44E9-82CE-CD20150D7111}"/>
     <hyperlink ref="B38" location="TC_037!A1" display="TC_037" xr:uid="{CDE51827-7D09-43FC-8E7C-238D0D06571C}"/>
+    <hyperlink ref="B39" location="TC_037!A1" display="TC_037" xr:uid="{F58394B0-769F-40CF-A949-4C557C0EB5B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15033,7 +15063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D645C1F-9493-4C45-B94F-D4B5A33B15C0}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
@@ -15082,7 +15112,7 @@
       </c>
       <c r="F4" s="30">
         <f ca="1">COUNTIFS(Summary!$D:$D,Statistics!F$3,Summary!$E:$E,Statistics!$D4)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="31">
         <f ca="1">COUNTIFS(Summary!$D:$D,Statistics!G$3,Summary!$E:$E,Statistics!$D4)</f>
@@ -15090,7 +15120,7 @@
       </c>
       <c r="H4" s="37">
         <f ca="1">SUM(E4:G4)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -15145,7 +15175,7 @@
       </c>
       <c r="F7" s="38">
         <f t="shared" ref="F7:G7" ca="1" si="1">SUM(F4:F6)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="39">
         <f t="shared" ca="1" si="1"/>
@@ -15153,7 +15183,7 @@
       </c>
       <c r="H7" s="41">
         <f ca="1">SUM(H4:H6)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -15599,34 +15629,34 @@
       </c>
       <c r="B63" s="69"/>
       <c r="C63" s="44">
-        <f>COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$D:$D,Statistics!C$52)</f>
+        <f ca="1">COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$D:$D,Statistics!C$52)</f>
         <v>0</v>
       </c>
       <c r="D63" s="9">
-        <f>COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$D:$D,Statistics!D$52)</f>
-        <v>0</v>
+        <f ca="1">COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$D:$D,Statistics!D$52)</f>
+        <v>1</v>
       </c>
       <c r="E63" s="43">
-        <f>COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$D:$D,Statistics!E$52)</f>
+        <f ca="1">COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$D:$D,Statistics!E$52)</f>
         <v>0</v>
       </c>
       <c r="F63" s="60"/>
       <c r="G63" s="44">
-        <f>COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$E:$E,Statistics!G$52)</f>
+        <f ca="1">COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$E:$E,Statistics!G$52)</f>
+        <v>1</v>
+      </c>
+      <c r="H63" s="9">
+        <f ca="1">COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$E:$E,Statistics!H$52)</f>
         <v>0</v>
       </c>
-      <c r="H63" s="9">
-        <f>COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$E:$E,Statistics!H$52)</f>
-        <v>0</v>
-      </c>
       <c r="I63" s="43">
-        <f>COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$E:$E,Statistics!I$52)</f>
+        <f ca="1">COUNTIFS(Summary!$A:$A,Statistics!$A63,Summary!$E:$E,Statistics!I$52)</f>
         <v>0</v>
       </c>
       <c r="J63" s="60"/>
       <c r="K63" s="62">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -25254,9 +25284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852F824F-45EC-4AE2-933B-67219A4D354F}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:D19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25444,7 +25472,9 @@
       <c r="C11" s="99"/>
       <c r="D11" s="100"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="92"/>
+      <c r="F11" s="92" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="94"/>
     </row>
@@ -25566,14 +25596,22 @@
       <c r="A19" s="9">
         <v>4</v>
       </c>
-      <c r="B19" s="110"/>
+      <c r="B19" s="110" t="s">
+        <v>305</v>
+      </c>
       <c r="C19" s="110"/>
       <c r="D19" s="110"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="119"/>
-      <c r="I19" s="9"/>
+      <c r="E19" s="116" t="s">
+        <v>306</v>
+      </c>
+      <c r="F19" s="117"/>
+      <c r="G19" s="116" t="s">
+        <v>306</v>
+      </c>
+      <c r="H19" s="117"/>
+      <c r="I19" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="J19" s="113"/>
       <c r="K19" s="113"/>
     </row>
@@ -25581,14 +25619,22 @@
       <c r="A20" s="9">
         <v>5</v>
       </c>
-      <c r="B20" s="110"/>
+      <c r="B20" s="110" t="s">
+        <v>307</v>
+      </c>
       <c r="C20" s="110"/>
       <c r="D20" s="110"/>
-      <c r="E20" s="114"/>
+      <c r="E20" s="114" t="s">
+        <v>308</v>
+      </c>
       <c r="F20" s="115"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="9"/>
+      <c r="G20" s="114" t="s">
+        <v>308</v>
+      </c>
+      <c r="H20" s="115"/>
+      <c r="I20" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="J20" s="113"/>
       <c r="K20" s="113"/>
     </row>

</xml_diff>